<commit_message>
Added footer and fixed semantic inconsistency
</commit_message>
<xml_diff>
--- a/documentatie/Beoordeling eindopdracht.xlsx
+++ b/documentatie/Beoordeling eindopdracht.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="46">
   <si>
     <t>De testtabel is aanwezig en ook qua structuur goed opgesteld in HTML/CSS</t>
   </si>
@@ -560,58 +560,58 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -954,31 +954,31 @@
       <c r="G2" s="5"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="40"/>
-      <c r="C3" s="40"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="40"/>
-      <c r="H3" s="41" t="e">
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="31" t="e">
         <f>CONCATENATE("Cijfer: ", B24)</f>
         <v>#REF!</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="39" t="s">
+      <c r="A4" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="42"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="32"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
@@ -997,16 +997,16 @@
       </c>
       <c r="B6" s="8"/>
       <c r="C6" s="9"/>
-      <c r="D6" s="43" t="s">
+      <c r="D6" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="44"/>
-      <c r="F6" s="44"/>
-      <c r="G6" s="44"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="34"/>
+      <c r="G6" s="34"/>
       <c r="H6" s="10"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="30" t="s">
+      <c r="A7" s="35" t="s">
         <v>13</v>
       </c>
       <c r="B7" s="11" t="s">
@@ -1016,16 +1016,16 @@
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="D7" s="33" t="s">
+      <c r="D7" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="34"/>
-      <c r="F7" s="34"/>
-      <c r="G7" s="34"/>
+      <c r="E7" s="39"/>
+      <c r="F7" s="39"/>
+      <c r="G7" s="39"/>
       <c r="H7" s="13"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="31"/>
+      <c r="A8" s="36"/>
       <c r="B8" s="11" t="s">
         <v>19</v>
       </c>
@@ -1033,14 +1033,14 @@
         <f>#REF!+#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="D8" s="35"/>
-      <c r="E8" s="36"/>
-      <c r="F8" s="36"/>
-      <c r="G8" s="36"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="41"/>
+      <c r="F8" s="41"/>
+      <c r="G8" s="41"/>
       <c r="H8" s="13"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="31"/>
+      <c r="A9" s="36"/>
       <c r="B9" s="11" t="s">
         <v>20</v>
       </c>
@@ -1048,14 +1048,14 @@
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="D9" s="35"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
-      <c r="G9" s="36"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="41"/>
+      <c r="G9" s="41"/>
       <c r="H9" s="13"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="32"/>
+      <c r="A10" s="37"/>
       <c r="B10" s="11" t="s">
         <v>17</v>
       </c>
@@ -1063,14 +1063,14 @@
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="D10" s="37"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="38"/>
-      <c r="G10" s="38"/>
+      <c r="D10" s="42"/>
+      <c r="E10" s="43"/>
+      <c r="F10" s="43"/>
+      <c r="G10" s="43"/>
       <c r="H10" s="14"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="30" t="s">
+      <c r="A11" s="35" t="s">
         <v>14</v>
       </c>
       <c r="B11" s="11" t="s">
@@ -1080,16 +1080,16 @@
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="D11" s="33" t="s">
+      <c r="D11" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
-      <c r="G11" s="34"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="39"/>
+      <c r="G11" s="39"/>
       <c r="H11" s="14"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="31"/>
+      <c r="A12" s="36"/>
       <c r="B12" s="11" t="s">
         <v>19</v>
       </c>
@@ -1097,14 +1097,14 @@
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="D12" s="35"/>
-      <c r="E12" s="36"/>
-      <c r="F12" s="36"/>
-      <c r="G12" s="36"/>
+      <c r="D12" s="40"/>
+      <c r="E12" s="41"/>
+      <c r="F12" s="41"/>
+      <c r="G12" s="41"/>
       <c r="H12" s="14"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="31"/>
+      <c r="A13" s="36"/>
       <c r="B13" s="11" t="s">
         <v>20</v>
       </c>
@@ -1112,14 +1112,14 @@
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="D13" s="35"/>
-      <c r="E13" s="36"/>
-      <c r="F13" s="36"/>
-      <c r="G13" s="36"/>
+      <c r="D13" s="40"/>
+      <c r="E13" s="41"/>
+      <c r="F13" s="41"/>
+      <c r="G13" s="41"/>
       <c r="H13" s="14"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="32"/>
+      <c r="A14" s="37"/>
       <c r="B14" s="11" t="s">
         <v>17</v>
       </c>
@@ -1127,14 +1127,14 @@
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="D14" s="37"/>
-      <c r="E14" s="38"/>
-      <c r="F14" s="38"/>
-      <c r="G14" s="38"/>
+      <c r="D14" s="42"/>
+      <c r="E14" s="43"/>
+      <c r="F14" s="43"/>
+      <c r="G14" s="43"/>
       <c r="H14" s="14"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="30" t="s">
+      <c r="A15" s="35" t="s">
         <v>15</v>
       </c>
       <c r="B15" s="11" t="s">
@@ -1144,16 +1144,16 @@
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="D15" s="33" t="s">
+      <c r="D15" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="E15" s="34"/>
-      <c r="F15" s="34"/>
-      <c r="G15" s="34"/>
+      <c r="E15" s="39"/>
+      <c r="F15" s="39"/>
+      <c r="G15" s="39"/>
       <c r="H15" s="14"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="31"/>
+      <c r="A16" s="36"/>
       <c r="B16" s="11" t="s">
         <v>19</v>
       </c>
@@ -1161,14 +1161,14 @@
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="D16" s="35"/>
-      <c r="E16" s="36"/>
-      <c r="F16" s="36"/>
-      <c r="G16" s="36"/>
+      <c r="D16" s="40"/>
+      <c r="E16" s="41"/>
+      <c r="F16" s="41"/>
+      <c r="G16" s="41"/>
       <c r="H16" s="14"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" s="31"/>
+      <c r="A17" s="36"/>
       <c r="B17" s="11" t="s">
         <v>20</v>
       </c>
@@ -1176,14 +1176,14 @@
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="D17" s="35"/>
-      <c r="E17" s="36"/>
-      <c r="F17" s="36"/>
-      <c r="G17" s="36"/>
+      <c r="D17" s="40"/>
+      <c r="E17" s="41"/>
+      <c r="F17" s="41"/>
+      <c r="G17" s="41"/>
       <c r="H17" s="14"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" s="32"/>
+      <c r="A18" s="37"/>
       <c r="B18" s="11" t="s">
         <v>17</v>
       </c>
@@ -1191,14 +1191,14 @@
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="D18" s="37"/>
-      <c r="E18" s="38"/>
-      <c r="F18" s="38"/>
-      <c r="G18" s="38"/>
+      <c r="D18" s="42"/>
+      <c r="E18" s="43"/>
+      <c r="F18" s="43"/>
+      <c r="G18" s="43"/>
       <c r="H18" s="14"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A19" s="30" t="s">
+      <c r="A19" s="35" t="s">
         <v>16</v>
       </c>
       <c r="B19" s="11" t="s">
@@ -1208,16 +1208,16 @@
         <f>Eindopdracht!C2</f>
         <v>4</v>
       </c>
-      <c r="D19" s="33" t="s">
+      <c r="D19" s="38" t="s">
         <v>29</v>
       </c>
-      <c r="E19" s="34"/>
-      <c r="F19" s="34"/>
-      <c r="G19" s="34"/>
+      <c r="E19" s="39"/>
+      <c r="F19" s="39"/>
+      <c r="G19" s="39"/>
       <c r="H19" s="14"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A20" s="31"/>
+      <c r="A20" s="36"/>
       <c r="B20" s="11" t="s">
         <v>19</v>
       </c>
@@ -1225,14 +1225,14 @@
         <f>Eindopdracht!C7</f>
         <v>5</v>
       </c>
-      <c r="D20" s="35"/>
-      <c r="E20" s="36"/>
-      <c r="F20" s="36"/>
-      <c r="G20" s="36"/>
+      <c r="D20" s="40"/>
+      <c r="E20" s="41"/>
+      <c r="F20" s="41"/>
+      <c r="G20" s="41"/>
       <c r="H20" s="14"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21" s="31"/>
+      <c r="A21" s="36"/>
       <c r="B21" s="11" t="s">
         <v>20</v>
       </c>
@@ -1240,14 +1240,14 @@
         <f>Eindopdracht!C13</f>
         <v>5</v>
       </c>
-      <c r="D21" s="35"/>
-      <c r="E21" s="36"/>
-      <c r="F21" s="36"/>
-      <c r="G21" s="36"/>
+      <c r="D21" s="40"/>
+      <c r="E21" s="41"/>
+      <c r="F21" s="41"/>
+      <c r="G21" s="41"/>
       <c r="H21" s="14"/>
     </row>
     <row r="22" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="32"/>
+      <c r="A22" s="37"/>
       <c r="B22" s="11" t="s">
         <v>17</v>
       </c>
@@ -1255,10 +1255,10 @@
         <f>Eindopdracht!C1</f>
         <v>10</v>
       </c>
-      <c r="D22" s="37"/>
-      <c r="E22" s="38"/>
-      <c r="F22" s="38"/>
-      <c r="G22" s="38"/>
+      <c r="D22" s="42"/>
+      <c r="E22" s="43"/>
+      <c r="F22" s="43"/>
+      <c r="G22" s="43"/>
       <c r="H22" s="14"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
@@ -1343,21 +1343,15 @@
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="24"/>
       <c r="B28" s="25"/>
-      <c r="C28" s="28"/>
-      <c r="D28" s="29"/>
-      <c r="E28" s="29"/>
-      <c r="F28" s="29"/>
-      <c r="G28" s="29"/>
+      <c r="C28" s="44"/>
+      <c r="D28" s="45"/>
+      <c r="E28" s="45"/>
+      <c r="F28" s="45"/>
+      <c r="G28" s="45"/>
       <c r="H28" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="H3:H4"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="D6:G6"/>
-    <mergeCell ref="A7:A10"/>
-    <mergeCell ref="D7:G10"/>
     <mergeCell ref="C28:G28"/>
     <mergeCell ref="A11:A14"/>
     <mergeCell ref="D11:G14"/>
@@ -1365,6 +1359,12 @@
     <mergeCell ref="D15:G18"/>
     <mergeCell ref="A19:A22"/>
     <mergeCell ref="D19:G22"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="D6:G6"/>
+    <mergeCell ref="A7:A10"/>
+    <mergeCell ref="D7:G10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1375,7 +1375,7 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1451,7 +1451,7 @@
       <c r="C6">
         <v>1</v>
       </c>
-      <c r="E6" s="45">
+      <c r="E6" s="28">
         <v>0.5</v>
       </c>
     </row>
@@ -1542,7 +1542,7 @@
         <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15" x14ac:dyDescent="0.2">
@@ -1552,6 +1552,9 @@
       <c r="C15">
         <v>1</v>
       </c>
+      <c r="E15" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="16" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
@@ -1559,6 +1562,9 @@
       </c>
       <c r="C16">
         <v>1</v>
+      </c>
+      <c r="E16" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="17" spans="2:3" ht="15" x14ac:dyDescent="0.2">

</xml_diff>